<commit_message>
Some results of chord analysis.
</commit_message>
<xml_diff>
--- a/chordGT/chord_k545.xlsx
+++ b/chordGT/chord_k545.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" tabRatio="500"/>
+    <workbookView xWindow="2800" yWindow="3320" windowWidth="25600" windowHeight="14580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="32">
   <si>
     <t>小節</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -146,6 +146,14 @@
   </si>
   <si>
     <t>備註</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ii</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -498,8 +506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F117"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="195" zoomScaleNormal="195" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A18" zoomScale="195" zoomScaleNormal="195" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -994,7 +1002,7 @@
         <v>11</v>
       </c>
       <c r="D29" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="E29">
         <v>6</v>
@@ -1028,7 +1036,7 @@
         <v>11</v>
       </c>
       <c r="D31" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="E31">
         <v>6</v>

</xml_diff>